<commit_message>
Refactoring, add frontTest and class
</commit_message>
<xml_diff>
--- a/Tests.xlsx
+++ b/Tests.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\A_Projects\C#\Cabinet_Maker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E75A1F8-5D72-43A9-8169-08F22427868D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFFCEC6-9323-4834-A98C-2D5C386914B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{DE3CEC85-4760-49A0-8B19-F244A0C33FDC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{DE3CEC85-4760-49A0-8B19-F244A0C33FDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Cabinet_Maker_Tests</t>
   </si>
@@ -208,6 +209,9 @@
   </si>
   <si>
     <t>Add_three_vertical_barrier_first_and_a_horizontal_to_the_four()</t>
+  </si>
+  <si>
+    <t>Kolejnosc tworzenia szafki</t>
   </si>
 </sst>
 </file>
@@ -258,12 +262,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -582,26 +585,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE8FA91B-A41A-4496-83B2-CC6C560DD27C}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
+    <sheetView topLeftCell="D25" workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="61.42578125" customWidth="1"/>
     <col min="4" max="4" width="87.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="C3" t="s">
@@ -615,8 +618,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
+      <c r="A4"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
@@ -628,10 +631,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>720</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -645,18 +648,18 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>600</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>510</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -670,10 +673,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -687,18 +690,18 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -712,10 +715,10 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -729,8 +732,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
+      <c r="A13"/>
+      <c r="B13" s="3"/>
       <c r="C13" s="1" t="s">
         <v>8</v>
       </c>
@@ -753,8 +756,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
+      <c r="A16"/>
+      <c r="B16" s="3"/>
       <c r="C16" s="1" t="s">
         <v>10</v>
       </c>
@@ -771,8 +774,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
+      <c r="A19"/>
+      <c r="B19" s="3"/>
       <c r="D19" s="1" t="s">
         <v>23</v>
       </c>
@@ -783,8 +786,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
+      <c r="A22"/>
+      <c r="B22" s="3"/>
       <c r="D22" s="1" t="s">
         <v>34</v>
       </c>
@@ -795,8 +798,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
+      <c r="A25"/>
+      <c r="B25" s="3"/>
       <c r="D25" s="1" t="s">
         <v>44</v>
       </c>
@@ -807,8 +810,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
+      <c r="A28"/>
+      <c r="B28" s="3"/>
       <c r="D28" s="1" t="s">
         <v>47</v>
       </c>
@@ -819,8 +822,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
+      <c r="A31"/>
+      <c r="B31" s="3"/>
       <c r="D31" s="1" t="s">
         <v>49</v>
       </c>
@@ -831,8 +834,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
+      <c r="A34"/>
+      <c r="B34" s="3"/>
       <c r="D34" s="1" t="s">
         <v>51</v>
       </c>
@@ -886,4 +889,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{573A139F-9802-4126-8245-05CC97AFB481}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>